<commit_message>
+ add repository tree ( + icons for Excel files, folders, PNG files) as QTreeWidget + fix some bags
</commit_message>
<xml_diff>
--- a/testtt.xlsx
+++ b/testtt.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <charset val="204"/>
@@ -41,6 +41,43 @@
       <charset val="204"/>
       <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="7"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,8 +107,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -452,10 +495,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C1" s="0" t="n">
@@ -466,10 +509,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>8</v>
       </c>
       <c r="C2" s="0" t="n">

</xml_diff>